<commit_message>
lotek srx800 alternative data format
</commit_message>
<xml_diff>
--- a/data/lotek fwfs.xlsx
+++ b/data/lotek fwfs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knebiolo\Desktop\Nuyakuk BIOTAS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kleinschmidtgroup-my.sharepoint.com/personal/kevin_nebiolo_kleinschmidtgroup_com/Documents/Software/biotas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C851D10-707D-4FDF-9DDE-2580DA08C881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{0C851D10-707D-4FDF-9DDE-2580DA08C881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCD9A0A-4286-4281-B7BC-AD838A5FE1B8}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5055" windowWidth="29040" windowHeight="15840" xr2:uid="{CAA84BEB-E981-4C85-B716-DA98EECC4265}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{CAA84BEB-E981-4C85-B716-DA98EECC4265}"/>
   </bookViews>
   <sheets>
     <sheet name="srx600 primary" sheetId="2" r:id="rId1"/>
     <sheet name="srx600 alternate" sheetId="1" r:id="rId2"/>
+    <sheet name="srx800 alternate" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="31">
   <si>
     <t>:</t>
   </si>
@@ -127,15 +128,25 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -171,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,7 +191,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BBCE7B-C88D-42B7-90EB-45E7326B53B9}">
   <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="AU3" sqref="AU3"/>
     </sheetView>
   </sheetViews>
@@ -724,32 +743,32 @@
         <v>15</v>
       </c>
       <c r="AI2" s="3"/>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" t="s">
         <v>16</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" t="s">
         <v>23</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AL2" t="s">
         <v>17</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AM2" t="s">
         <v>18</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AN2" t="s">
         <v>23</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AO2" t="s">
         <v>23</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AP2" t="s">
         <v>16</v>
       </c>
       <c r="AQ2" s="3"/>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" t="s">
         <v>26</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AS2" t="s">
         <v>27</v>
       </c>
       <c r="AT2" t="s">
@@ -850,7 +869,7 @@
   <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1"/>
+      <selection sqref="A1:AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,4 +1124,404 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE100EB4-E4D8-481F-9C3B-EA4F699A395C}">
+  <dimension ref="A1:BB3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection sqref="A1:BA1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:54" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="4">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4">
+        <v>18</v>
+      </c>
+      <c r="T1" s="4">
+        <v>19</v>
+      </c>
+      <c r="U1" s="4">
+        <v>20</v>
+      </c>
+      <c r="V1" s="4">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="4">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="4">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="4">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="4">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="4">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="4">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="4">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="4">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="4">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="4">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="4">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="4">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="4">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="4">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="4">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="4">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="4">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="4">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="4">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="4">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="4">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="4">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="4">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="4">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="4">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="4">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="4">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="4">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="6"/>
+      <c r="AN2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU2" s="6"/>
+      <c r="AV2" s="6"/>
+      <c r="AW2" s="6"/>
+      <c r="AX2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="BA2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="BB2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="4">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>5</v>
+      </c>
+      <c r="K3" s="4">
+        <v>8</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>5</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="5">
+        <v>0</v>
+      </c>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4">
+        <v>9</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>9</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>9</v>
+      </c>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6"/>
+      <c r="AM3" s="6"/>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="6"/>
+      <c r="AV3" s="6"/>
+      <c r="AW3" s="6"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="4">
+        <v>6</v>
+      </c>
+      <c r="BB3" s="5">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>